<commit_message>
Richiesta accreditamento dopo fix segnalazioni
Effettuati fix aitest [448, 449] segnalati tramite mail
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#BRAINSIXSRLXX/BrainSix/CMF_FSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#BRAINSIXSRLXX/BrainSix/CMF_FSE/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrogriggio/Documents/Docker/CMF/[TestCaseFSE]/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E930EA23-E8A4-D04B-9A1E-657AE6BDC734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F20653E-2DB7-8944-BE4C-F9548D8ABB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -799,28 +799,28 @@
     <t>VALIDAZIONE_RSA_TIMEOUT+H29D12+H+D12</t>
   </si>
   <si>
-    <t>2025-10-30T08:21:15.898+01:00</t>
-  </si>
-  <si>
-    <t>da2e5156f89bdea31f83b24b744d3224</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.999.d53158df5b51c17f1cf442a1d3bfd70badaecfbce24e871d7859ef35aa051500.456145375b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-30T08:23:14.015+01:00</t>
-  </si>
-  <si>
-    <t>3e0f5ca3412f2625ccaf9fb9738a9595</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.999.a775db011a5d69098547f811359b317a43043f4e1cad81876f4b2b612f4cbfbd.c7b6d4dd06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>BrainSix Srl</t>
   </si>
   <si>
     <t>2025-10-29T14:19:11.963+01:00</t>
+  </si>
+  <si>
+    <t>2025-11-04T20:33:27.962+01:00</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.999.1d973a8e136eacef1c74db74a74381191fd70c7b4b98326e124a1dba6c3bd4b0.cd30d08c31^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>77b71af40db49668114fddcc893aba82</t>
+  </si>
+  <si>
+    <t>050f3d1088d509821c34299779a5fa39</t>
+  </si>
+  <si>
+    <t>2025-11-04T20:36:01.643+01:00</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.999.5bc26441657726392edf3f90cb7ea212a3871d549ebd016aef2ff1da499a7e6d.62c2579d75^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2875,10 +2875,10 @@
   <dimension ref="A1:W592"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="B2" s="46"/>
       <c r="C2" s="47" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D2" s="46"/>
       <c r="F2" s="6"/>
@@ -3244,7 +3244,7 @@
         <v>45959</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H11" s="32" t="s">
         <v>120</v>
@@ -4126,16 +4126,16 @@
         <v>97</v>
       </c>
       <c r="F28" s="32">
-        <v>45960</v>
+        <v>45965</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H28" s="32" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I28" s="37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>42</v>
@@ -4173,16 +4173,16 @@
         <v>98</v>
       </c>
       <c r="F29" s="32">
-        <v>45960</v>
+        <v>45965</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>42</v>
@@ -10497,6 +10497,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10754,28 +10775,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10794,31 +10819,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Richiesta accreditamento dopo fix segnalazioni #2
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#BRAINSIXSRLXX/BrainSix/CMF_FSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#BRAINSIXSRLXX/BrainSix/CMF_FSE/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrogriggio/Documents/Docker/CMF/[TestCaseFSE]/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F20653E-2DB7-8944-BE4C-F9548D8ABB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DD7F29-3AD1-7549-815A-57E317A3911D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -814,13 +814,13 @@
     <t>77b71af40db49668114fddcc893aba82</t>
   </si>
   <si>
-    <t>050f3d1088d509821c34299779a5fa39</t>
-  </si>
-  <si>
-    <t>2025-11-04T20:36:01.643+01:00</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.999.5bc26441657726392edf3f90cb7ea212a3871d549ebd016aef2ff1da499a7e6d.62c2579d75^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-06T16:43:29.793+01:00</t>
+  </si>
+  <si>
+    <t>ef16cd5b1a5fd3b8f91c662ab661be6f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.999.f8075feaec98c882237f3f2ba13815340b884a2db681015d975397306fc2e538.0d277bcf46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4173,13 +4173,13 @@
         <v>98</v>
       </c>
       <c r="F29" s="32">
-        <v>45965</v>
+        <v>45967</v>
       </c>
       <c r="G29" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="H29" s="32" t="s">
         <v>187</v>
-      </c>
-      <c r="H29" s="32" t="s">
-        <v>186</v>
       </c>
       <c r="I29" s="37" t="s">
         <v>188</v>
@@ -10497,27 +10497,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10775,32 +10754,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10819,6 +10794,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Compilazione colonne Q e R per casi segnalati via mail
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#BRAINSIXSRLXX/BrainSix/CMF_FSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#BRAINSIXSRLXX/BrainSix/CMF_FSE/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrogriggio/Documents/Docker/CMF/[TestCaseFSE]/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DD7F29-3AD1-7549-815A-57E317A3911D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AC86C8-8626-DB47-9171-A7EAA9BA6B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="189">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2875,10 +2875,10 @@
   <dimension ref="A1:W592"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3210,8 +3210,12 @@
       <c r="P10" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
+      <c r="Q10" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R10" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S10" s="33" t="s">
         <v>119</v>
       </c>
@@ -3269,8 +3273,12 @@
       <c r="P11" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
+      <c r="Q11" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R11" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S11" s="33" t="s">
         <v>119</v>
       </c>
@@ -3381,8 +3389,12 @@
       <c r="P13" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="33"/>
+      <c r="Q13" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R13" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S13" s="33" t="s">
         <v>119</v>
       </c>
@@ -3440,8 +3452,12 @@
       <c r="P14" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
+      <c r="Q14" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R14" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S14" s="33" t="s">
         <v>119</v>
       </c>
@@ -3499,8 +3515,12 @@
       <c r="P15" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
+      <c r="Q15" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R15" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S15" s="33" t="s">
         <v>119</v>
       </c>
@@ -3558,8 +3578,12 @@
       <c r="P16" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
+      <c r="Q16" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R16" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S16" s="33" t="s">
         <v>119</v>
       </c>
@@ -3617,8 +3641,12 @@
       <c r="P17" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
+      <c r="Q17" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R17" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S17" s="33" t="s">
         <v>119</v>
       </c>
@@ -3676,8 +3704,12 @@
       <c r="P18" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
+      <c r="Q18" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R18" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S18" s="33" t="s">
         <v>119</v>
       </c>
@@ -3735,8 +3767,12 @@
       <c r="P19" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
+      <c r="Q19" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R19" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S19" s="33" t="s">
         <v>119</v>
       </c>
@@ -3831,8 +3867,12 @@
       <c r="P21" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
+      <c r="Q21" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R21" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S21" s="33" t="s">
         <v>119</v>
       </c>
@@ -4095,8 +4135,12 @@
       <c r="P27" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
+      <c r="Q27" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R27" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S27" s="33" t="s">
         <v>119</v>
       </c>
@@ -4289,8 +4333,12 @@
       <c r="P31" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="33"/>
+      <c r="Q31" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R31" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S31" s="33" t="s">
         <v>119</v>
       </c>
@@ -4348,8 +4396,12 @@
       <c r="P32" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="33"/>
+      <c r="Q32" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R32" s="33" t="s">
+        <v>42</v>
+      </c>
       <c r="S32" s="33" t="s">
         <v>119</v>
       </c>
@@ -8360,7 +8412,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Q20:R21 P21 P10:R19 J10:J21 J27:J32 P22:R32 M10:N32</xm:sqref>
+          <xm:sqref>R10:R20 M10:N32 J10:J21 J27:J32 Q20 P10:Q19 P21:R32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE61C5E-9DA3-4CE3-A1FF-8FBE651EA6B5}">
           <x14:formula1>
@@ -10497,6 +10549,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -10754,28 +10827,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10794,31 +10871,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>